<commit_message>
cambios traslados y desvinculacion
</commit_message>
<xml_diff>
--- a/configs/gestion-config/assets/excel-ejemplos/jornada.xlsx
+++ b/configs/gestion-config/assets/excel-ejemplos/jornada.xlsx
@@ -1,33 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\tickets-soporte\configs\gestion-config\assets\excel-ejemplos\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AED445B-F626-4742-B64A-4D103B622334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Tipo de Jornada</t>
-  </si>
-  <si>
-    <t>Hora entrada</t>
-  </si>
-  <si>
-    <t>Hora salida</t>
   </si>
   <si>
     <t>Jornada 1</t>
@@ -39,8 +34,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -69,7 +64,13 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -86,6 +87,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -94,10 +103,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -373,42 +382,40 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C5" sqref="B1:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.135" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.57031" customWidth="1"/>
-    <col min="3" max="3" width="26.85547" customWidth="1"/>
-    <col min="4" max="4" width="29.707" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.137" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.564" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.135" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.565" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.565" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.283" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="31.135" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.566" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" customWidth="1"/>
+    <col min="4" max="4" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="30" customHeight="1">
+    <row r="1" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -419,28 +426,21 @@
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
-      <c r="B2" s="2">
-        <v>0.33333333333333326</v>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
       </c>
-      <c r="C2" s="2">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2">
-        <v>0.75</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0.33333333333333326</v>
-      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>